<commit_message>
Deployed d6b98274 to 2024.02.01 with MkDocs 1.5.3 and mike 2.0.0
</commit_message>
<xml_diff>
--- a/2024.02.01/DSP-TOOLS/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
+++ b/2024.02.01/DSP-TOOLS/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/docs/assets/data_model_templates/rosetta (rosetta)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D486172C-7999-6645-BB1D-EBFA2158D7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADD7F20-3DF7-0F4F-A598-8DFEF1279E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="3600" windowWidth="27640" windowHeight="16940" xr2:uid="{39EADD64-DA63-9448-899F-8078B27ECEBC}"/>
+    <workbookView xWindow="22520" yWindow="5660" windowWidth="27640" windowHeight="16940" xr2:uid="{39EADD64-DA63-9448-899F-8078B27ECEBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -263,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{D3FBF9CF-C152-F14C-BAC2-96F9D75C9E8D}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{D3FBF9CF-C152-F14C-BAC2-96F9D75C9E8D}">
       <text>
         <r>
           <rPr>
@@ -316,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{3FCB58FD-3EA0-D649-A225-B6DF2A08C021}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{3FCB58FD-3EA0-D649-A225-B6DF2A08C021}">
       <text>
         <r>
           <rPr>
@@ -374,7 +373,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="152">
   <si>
     <t>label_de</t>
   </si>
@@ -827,6 +826,9 @@
   </si>
   <si>
     <t>Number of children</t>
+  </si>
+  <si>
+    <t>subject</t>
   </si>
 </sst>
 </file>
@@ -1213,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C6BB55-8531-3D43-8AA9-4A28D8869FE7}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1232,11 +1234,12 @@
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
+    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>104</v>
       </c>
@@ -1277,13 +1280,16 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -1302,14 +1308,14 @@
       <c r="M2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>17</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>106</v>
       </c>
@@ -1328,14 +1334,14 @@
       <c r="M3" t="s">
         <v>22</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>23</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -1354,14 +1360,14 @@
       <c r="M4" t="s">
         <v>27</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>28</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1380,11 +1386,11 @@
       <c r="M5" t="s">
         <v>33</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>108</v>
       </c>
@@ -1403,11 +1409,11 @@
       <c r="M6" t="s">
         <v>22</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -1426,14 +1432,14 @@
       <c r="M7" t="s">
         <v>22</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>23</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -1452,14 +1458,14 @@
       <c r="M8" t="s">
         <v>16</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>17</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>111</v>
       </c>
@@ -1478,11 +1484,11 @@
       <c r="M9" t="s">
         <v>46</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -1501,11 +1507,11 @@
       <c r="M10" t="s">
         <v>22</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -1524,11 +1530,11 @@
       <c r="M11" t="s">
         <v>52</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -1547,11 +1553,11 @@
       <c r="M12" t="s">
         <v>55</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>115</v>
       </c>
@@ -1570,14 +1576,14 @@
       <c r="M13" t="s">
         <v>27</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>58</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>116</v>
       </c>
@@ -1596,14 +1602,14 @@
       <c r="M14" t="s">
         <v>62</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>17</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -1622,14 +1628,14 @@
       <c r="M15" t="s">
         <v>22</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>23</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -1648,11 +1654,11 @@
       <c r="M16" t="s">
         <v>55</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>119</v>
       </c>
@@ -1671,14 +1677,14 @@
       <c r="M17" t="s">
         <v>22</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>23</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -1697,11 +1703,11 @@
       <c r="M18" t="s">
         <v>22</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>121</v>
       </c>
@@ -1720,14 +1726,14 @@
       <c r="M19" t="s">
         <v>74</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>17</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>122</v>
       </c>
@@ -1746,11 +1752,11 @@
       <c r="M20" t="s">
         <v>77</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>123</v>
       </c>
@@ -1769,11 +1775,11 @@
       <c r="M21" t="s">
         <v>22</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>124</v>
       </c>
@@ -1792,11 +1798,11 @@
       <c r="M22" t="s">
         <v>22</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -1815,11 +1821,11 @@
       <c r="M23" t="s">
         <v>22</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -1838,11 +1844,11 @@
       <c r="M24" t="s">
         <v>22</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>127</v>
       </c>
@@ -1861,14 +1867,14 @@
       <c r="M25" t="s">
         <v>89</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>23</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -1887,14 +1893,14 @@
       <c r="M26" t="s">
         <v>93</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>17</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -1913,11 +1919,11 @@
       <c r="M27" t="s">
         <v>96</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -1936,14 +1942,14 @@
       <c r="M28" t="s">
         <v>52</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>23</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>131</v>
       </c>
@@ -1962,10 +1968,10 @@
       <c r="M29" t="s">
         <v>101</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>102</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1974,12 +1980,13 @@
     <hyperlink ref="G1" r:id="rId1" location="property-comments" xr:uid="{C5745B79-2350-9040-A33B-B990DB1FB220}"/>
     <hyperlink ref="L1" r:id="rId2" location="property-super" xr:uid="{C93CACE1-16EA-C64C-B3B5-98BAC468E60A}"/>
     <hyperlink ref="M1" r:id="rId3" location="property-object-gui_element-gui_attributes" xr:uid="{A404F957-34EE-1C45-84B6-64764F3311EA}"/>
-    <hyperlink ref="N1" r:id="rId4" location="property-object-gui_element-gui_attributes" xr:uid="{B488EDE5-F9B6-D249-9B67-4BD8C52BD8DF}"/>
-    <hyperlink ref="O1" r:id="rId5" location="property-object-gui_element-gui_attributes" xr:uid="{A3CD059E-237B-BC4D-A227-4194429C8852}"/>
+    <hyperlink ref="O1" r:id="rId4" location="property-object-gui_element-gui_attributes" xr:uid="{B488EDE5-F9B6-D249-9B67-4BD8C52BD8DF}"/>
+    <hyperlink ref="P1" r:id="rId5" location="property-object-gui_element-gui_attributes" xr:uid="{A3CD059E-237B-BC4D-A227-4194429C8852}"/>
     <hyperlink ref="A1" r:id="rId6" location="property-name" xr:uid="{49D9B3A1-289C-AD44-A8C7-AFCC3397B32D}"/>
     <hyperlink ref="B1" r:id="rId7" location="property-labels" xr:uid="{1C4C342B-22AD-2440-901D-5A8E98EBE39C}"/>
+    <hyperlink ref="N1" r:id="rId8" location="property-subject" xr:uid="{556249D5-670B-2E4F-AD37-1A7B1463E00F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>